<commit_message>
changements sur le projet / passage à l'interconnexion entre les objets connectés type smartwatch
</commit_message>
<xml_diff>
--- a/smartfridge_budget.xlsx
+++ b/smartfridge_budget.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,29 +436,29 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Category</t>
+          <t>Catégorie</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Description</t>
+          <t>Détail</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Estimated Cost (€)</t>
+          <t>Coût estimé (€)</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Hardware</t>
+          <t>Prototype matériel</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Fridge, cameras, Jetson Nano</t>
+          <t>Frigo modifié + caméras + module IA embarqué</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -468,12 +468,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Software</t>
+          <t>Développement logiciel</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Development tools &amp; frameworks</t>
+          <t>App mobile, backend FastAPI, intégration Drive</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -483,12 +483,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Human Resources</t>
+          <t>Ressources humaines (IA / IoT / Mobile / Backend)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>IA, IoT, Mobile developers</t>
+          <t>1 mois de travail cumulé des rôles clés</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -498,12 +498,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Infrastructure</t>
+          <t>Infra Cloud (hébergement API / DB)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Cloud server &amp; storage</t>
+          <t>Serveur OVH/AWS + stockage données 1 an</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -513,42 +513,57 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Training</t>
+          <t>Tests terrain / panels utilisateurs</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>AI model training</t>
+          <t>Séances de tests en conditions réelles</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Miscellaneous</t>
+          <t>Communication / gouvernance projet</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Meetings, communication, contingency</t>
+          <t>Réunions projet, doc, pilotage PO</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>500</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>Marge imprévus (10%)</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Buffer sécurité budget matériel / délai fournisseur</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="n">
-        <v>6500</v>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="n">
+        <v>6820</v>
       </c>
     </row>
   </sheetData>

</xml_diff>